<commit_message>
Punkt 2 in Labor 16
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598B0242-C50F-499C-A51B-2C104BF1B835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F760DD1-85AB-434D-86F8-3CB92B87F2B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="28">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1911,7 +1911,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2091,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>4</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="20">
-        <f t="shared" si="0"/>
+        <f>(D9-C9)*24*60 - E9</f>
         <v>349.99999999999983</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -2120,27 +2120,57 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7">
+        <v>43519</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.51388888888888895</v>
+      </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="F10" s="20">
+        <f>(D10-C10)*24*60 - E10</f>
+        <v>170.00000000000011</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="9">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43519</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.86805555555555547</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="F11" s="5">
+        <f>(D11-C11)*24*60 - E11</f>
+        <v>160.00000000000006</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>27</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="10"/>
     </row>
@@ -2166,7 +2196,7 @@
       <c r="E13" s="31"/>
       <c r="F13" s="25">
         <f>SUM(F6:F12)</f>
-        <v>630</v>
+        <v>960.00000000000023</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>

</xml_diff>

<commit_message>
Created the "create, read, update and delete"
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CEA79B-3053-4AA8-8692-EB14B18EAC5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37272A74-8C77-4A45-8FE4-59A42F1C5C02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
     <sheet name="Nädal 2" sheetId="2" r:id="rId2"/>
     <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="31">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -120,6 +121,12 @@
   </si>
   <si>
     <t>Praktikum</t>
+  </si>
+  <si>
+    <t>Proge.</t>
+  </si>
+  <si>
+    <t>MVC EF</t>
   </si>
 </sst>
 </file>
@@ -604,84 +611,84 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1017,68 +1024,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="56">
         <v>43493</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="57"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1354,13 +1361,13 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="42"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="25">
         <f>SUM(F7:F15)</f>
         <v>900.99999999999989</v>
@@ -1401,68 +1408,68 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="45"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="49" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="56">
         <v>43500</v>
       </c>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="57"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1685,13 +1692,13 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="25">
         <f>SUM(F7:F13)</f>
         <v>912.00000000000023</v>
@@ -1730,68 +1737,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="56">
         <v>43507</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
@@ -2013,13 +2020,13 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="25">
         <f>SUM(F6:F12)</f>
         <v>1008.9999999999999</v>
@@ -2048,8 +2055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D31881A-EB86-4A93-9BC9-AEBD141C84F9}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,68 +2066,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="48"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="56">
         <v>43514</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="51"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="54"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="61"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="34" t="s">
         <v>4</v>
       </c>
@@ -2344,35 +2351,35 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="62">
+      <c r="A13" s="38">
         <v>8</v>
       </c>
-      <c r="B13" s="63">
+      <c r="B13" s="39">
         <v>43519</v>
       </c>
-      <c r="C13" s="64">
+      <c r="C13" s="40">
         <v>0.86805555555555547</v>
       </c>
-      <c r="D13" s="64">
+      <c r="D13" s="40">
         <v>1</v>
       </c>
-      <c r="E13" s="62">
+      <c r="E13" s="38">
         <v>10</v>
       </c>
-      <c r="F13" s="65">
+      <c r="F13" s="41">
         <f>(D13-C13)*24*60 - E13</f>
         <v>180.00000000000011</v>
       </c>
-      <c r="G13" s="62" t="s">
+      <c r="G13" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="66" t="s">
+      <c r="H13" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-    </row>
-    <row r="14" spans="1:10" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>9</v>
       </c>
@@ -2400,13 +2407,13 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
       <c r="F15" s="27">
         <f>SUM(F6:F14)</f>
         <v>1425.0000000000005</v>
@@ -2429,4 +2436,260 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C756A1-99A3-4432-BBB5-58650AF383D0}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="56">
+        <v>43521</v>
+      </c>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="67"/>
+      <c r="C5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>43522</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.84583333333333333</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F8" si="0">(D6-C6)*24*60 - E6</f>
+        <v>138</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="27">
+        <f>SUM(F6:F14)</f>
+        <v>138</v>
+      </c>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created an enitial migration
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37272A74-8C77-4A45-8FE4-59A42F1C5C02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F9426-4525-4C46-BD1C-A4C5057E056C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="31">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2443,7 +2443,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,26 +2568,56 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43523</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.56944444444444442</v>
+      </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="30"/>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>79.999999999999872</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43523</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="30"/>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>119.99999999999989</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
@@ -2673,7 +2703,7 @@
       <c r="E15" s="65"/>
       <c r="F15" s="27">
         <f>SUM(F6:F14)</f>
-        <v>138</v>
+        <v>337.99999999999977</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>

</xml_diff>

<commit_message>
Add attributes and changed SQL tabel
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F9426-4525-4C46-BD1C-A4C5057E056C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24674D86-54B1-44E2-BAC0-172F6C557A5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="31">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2443,7 +2443,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5">
-        <f t="shared" ref="F6:F8" si="0">(D6-C6)*24*60 - E6</f>
+        <f t="shared" ref="F6:F9" si="0">(D6-C6)*24*60 - E6</f>
         <v>138</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -2622,14 +2622,31 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="30"/>
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43524</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="E9" s="6">
+        <v>30</v>
+      </c>
+      <c r="F9" s="5">
+        <f>(D9-C9)*24*60 - E9</f>
+        <v>265.00000000000006</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
@@ -2703,7 +2720,7 @@
       <c r="E15" s="65"/>
       <c r="F15" s="27">
         <f>SUM(F6:F14)</f>
-        <v>337.99999999999977</v>
+        <v>602.99999999999977</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>

</xml_diff>

<commit_message>
Seed database with test data
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24674D86-54B1-44E2-BAC0-172F6C557A5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05943642-E79E-4FBE-8C82-2BF0AAB22D84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="31">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="A1:K13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,7 +2443,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5">
-        <f t="shared" ref="F6:F9" si="0">(D6-C6)*24*60 - E6</f>
+        <f t="shared" ref="F6:F8" si="0">(D6-C6)*24*60 - E6</f>
         <v>138</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -2651,26 +2651,58 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="33"/>
+      <c r="A10" s="31">
+        <v>5</v>
+      </c>
+      <c r="B10" s="32">
+        <v>43525</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E10" s="6">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5">
+        <f>(D10-C10)*24*60 - E10</f>
+        <v>165</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>28</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="31">
+        <v>6</v>
+      </c>
+      <c r="B11" s="32">
+        <v>43526</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="33"/>
+      <c r="F11" s="5">
+        <f>(D11-C11)*24*60 - E11</f>
+        <v>99.999999999999886</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>30</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
@@ -2720,7 +2752,7 @@
       <c r="E15" s="65"/>
       <c r="F15" s="27">
         <f>SUM(F6:F14)</f>
-        <v>602.99999999999977</v>
+        <v>867.99999999999966</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>

</xml_diff>

<commit_message>
Now migrations works normaly
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05943642-E79E-4FBE-8C82-2BF0AAB22D84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F4BAE5-7D4A-4F87-AE02-538959C7EEDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="32">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>MVC EF</t>
+  </si>
+  <si>
+    <t>Book</t>
   </si>
 </sst>
 </file>
@@ -2443,7 +2446,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,16 +2710,33 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43527</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.93402777777777779</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="30"/>
+      <c r="F12" s="5">
+        <f>(D12-C12)*24*60 - E12</f>
+        <v>135</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>31</v>
+      </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
@@ -2752,7 +2772,7 @@
       <c r="E15" s="65"/>
       <c r="F15" s="27">
         <f>SUM(F6:F14)</f>
-        <v>867.99999999999966</v>
+        <v>1002.9999999999997</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>

</xml_diff>

<commit_message>
SQL tabelis on kõik asjad, mis on vaja
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F4BAE5-7D4A-4F87-AE02-538959C7EEDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F55E2D-22B4-49DD-A907-FF6990546082}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
     <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="34">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -130,6 +131,12 @@
   </si>
   <si>
     <t>Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class </t>
+  </si>
+  <si>
+    <t>Proge</t>
   </si>
 </sst>
 </file>
@@ -2445,8 +2452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C756A1-99A3-4432-BBB5-58650AF383D0}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,4 +2798,379 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89E0861-BAB8-4604-8D41-66920099459A}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="54"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="62"/>
+      <c r="C3" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="56">
+        <v>43528</v>
+      </c>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="57"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="58"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="60"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="67"/>
+      <c r="C5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>43528</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="5">
+        <f t="shared" ref="F6:F13" si="0">(D6-C6)*24*60 - E6</f>
+        <v>90</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43529</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E7" s="6">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>230.00000000000011</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43529</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>120.00000000000006</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43530</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="E9" s="6">
+        <v>20</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>219.99999999999994</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>5</v>
+      </c>
+      <c r="B10" s="32">
+        <v>43531</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="E10" s="6">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>140.00000000000003</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
+        <v>6</v>
+      </c>
+      <c r="B11" s="32">
+        <v>43531</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E11" s="6">
+        <v>20</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>119.99999999999983</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43531</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.6875</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="E12" s="6">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>179.99999999999994</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>8</v>
+      </c>
+      <c r="B13" s="39">
+        <v>43531</v>
+      </c>
+      <c r="C13" s="40">
+        <v>0.875</v>
+      </c>
+      <c r="D13" s="40">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E13" s="38">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>134.99999999999994</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="38"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="27">
+        <f>SUM(F6:F14)</f>
+        <v>1235</v>
+      </c>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Start the new week
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F55E2D-22B4-49DD-A907-FF6990546082}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9062D425-1C52-4435-B954-CBC45F13C829}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="34">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2802,15 +2802,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89E0861-BAB8-4604-8D41-66920099459A}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2916,7 +2917,7 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5">
-        <f t="shared" ref="F6:F13" si="0">(D6-C6)*24*60 - E6</f>
+        <f t="shared" ref="F6:F15" si="0">(D6-C6)*24*60 - E6</f>
         <v>90</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -3132,37 +3133,110 @@
       <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="31">
+        <v>9</v>
+      </c>
+      <c r="B14" s="32">
+        <v>43532</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.4375</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="30"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>150.00000000000003</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
+        <v>10</v>
+      </c>
+      <c r="B15" s="32">
+        <v>43532</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="E15" s="6">
+        <v>30</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>250.00000000000006</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>11</v>
+      </c>
+      <c r="B16" s="32">
+        <v>43532</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="5">
+        <f t="shared" ref="F16" si="1">(D16-C16)*24*60 - E16</f>
+        <v>80.000000000000028</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="27">
-        <f>SUM(F6:F14)</f>
-        <v>1235</v>
-      </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="27">
+        <f>SUM(F6:F16)</f>
+        <v>1715</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>

</xml_diff>

<commit_message>
Update the Delete page
</commit_message>
<xml_diff>
--- a/Logs/Logs_Vladislav_Jekimtsev.xlsx
+++ b/Logs/Logs_Vladislav_Jekimtsev.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekimt\source\repos\ISA2_Vladislav_Jekimtsev\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991E0BAB-F37A-47B0-BF08-B2B828F20AE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3EF3F6-E0A9-492D-AB01-B2A6C6C6E466}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="35">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -3258,7 +3258,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3412,16 +3412,28 @@
       <c r="A8" s="6">
         <v>3</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="7">
+        <v>43537</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E8" s="6">
+        <v>20</v>
+      </c>
       <c r="F8" s="5">
         <f>(D8-C8)*24*60 - E8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="30"/>
+        <v>420.00000000000006</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
@@ -3571,7 +3583,7 @@
       <c r="E17" s="65"/>
       <c r="F17" s="27">
         <f>SUM(F6:F16)</f>
-        <v>149.99999999999994</v>
+        <v>570</v>
       </c>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>

</xml_diff>